<commit_message>
New Sheets Alert! participatingAgencies08122025pm.xlsx and pendingAgencies08122025pm.xlsx
</commit_message>
<xml_diff>
--- a/Pivot PendingAgencies/pivot-pendingAgencies08122025pm.xlsx
+++ b/Pivot PendingAgencies/pivot-pendingAgencies08122025pm.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,11 +450,6 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>New</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>Present</t>
         </is>
       </c>
@@ -471,9 +466,6 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -485,9 +477,6 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -503,9 +492,6 @@
       <c r="C4" t="n">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -519,9 +505,6 @@
       <c r="C5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -535,9 +518,6 @@
       <c r="C6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -549,9 +529,6 @@
         <v>114</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
         <v>2</v>
       </c>
     </row>
@@ -565,9 +542,6 @@
         <v>22</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -583,9 +557,6 @@
       <c r="C9" t="n">
         <v>2</v>
       </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -599,9 +570,6 @@
       <c r="C10" t="n">
         <v>0</v>
       </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -615,9 +583,6 @@
       <c r="C11" t="n">
         <v>0</v>
       </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -631,9 +596,6 @@
       <c r="C12" t="n">
         <v>0</v>
       </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -647,9 +609,6 @@
       <c r="C13" t="n">
         <v>0</v>
       </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -661,9 +620,6 @@
         <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
         <v>2</v>
       </c>
     </row>
@@ -679,9 +635,6 @@
       <c r="C15" t="n">
         <v>0</v>
       </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -695,9 +648,6 @@
       <c r="C16" t="n">
         <v>0</v>
       </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -711,9 +661,6 @@
       <c r="C17" t="n">
         <v>0</v>
       </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -727,9 +674,6 @@
       <c r="C18" t="n">
         <v>0</v>
       </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -743,9 +687,6 @@
       <c r="C19" t="n">
         <v>0</v>
       </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -759,9 +700,6 @@
       <c r="C20" t="n">
         <v>0</v>
       </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -775,9 +713,6 @@
       <c r="C21" t="n">
         <v>0</v>
       </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -791,9 +726,6 @@
       <c r="C22" t="n">
         <v>0</v>
       </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -805,9 +737,6 @@
         <v>4</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -823,9 +752,6 @@
       <c r="C24" t="n">
         <v>0</v>
       </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -839,9 +765,6 @@
       <c r="C25" t="n">
         <v>0</v>
       </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -855,9 +778,6 @@
       <c r="C26" t="n">
         <v>0</v>
       </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -871,9 +791,6 @@
       <c r="C27" t="n">
         <v>0</v>
       </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -887,9 +804,6 @@
       <c r="C28" t="n">
         <v>0</v>
       </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -903,9 +817,6 @@
       <c r="C29" t="n">
         <v>0</v>
       </c>
-      <c r="D29" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -917,9 +828,6 @@
         <v>8</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="n">
         <v>1</v>
       </c>
     </row>
@@ -933,10 +841,7 @@
         <v>25</v>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
-      </c>
-      <c r="D31" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
@@ -951,9 +856,6 @@
       <c r="C32" t="n">
         <v>0</v>
       </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -967,9 +869,6 @@
       <c r="C33" t="n">
         <v>1</v>
       </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -983,9 +882,6 @@
       <c r="C34" t="n">
         <v>0</v>
       </c>
-      <c r="D34" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -997,9 +893,6 @@
         <v>15</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1013,9 +906,6 @@
         <v>61</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="n">
         <v>11</v>
       </c>
     </row>
@@ -1031,9 +921,6 @@
       <c r="C37" t="n">
         <v>0</v>
       </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1045,9 +932,6 @@
         <v>17</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1063,9 +947,6 @@
       <c r="C39" t="n">
         <v>0</v>
       </c>
-      <c r="D39" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1077,9 +958,6 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1095,9 +973,6 @@
       <c r="C41" t="n">
         <v>0</v>
       </c>
-      <c r="D41" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1111,9 +986,6 @@
       <c r="C42" t="n">
         <v>0</v>
       </c>
-      <c r="D42" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1125,10 +997,7 @@
         <v>429</v>
       </c>
       <c r="C43" t="n">
-        <v>6</v>
-      </c>
-      <c r="D43" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>